<commit_message>
ManualPreprocessing and SK_preprocessing scripts
</commit_message>
<xml_diff>
--- a/Matt/LabelledVar.xlsx
+++ b/Matt/LabelledVar.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15060" yWindow="40" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17940" windowHeight="18700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="83">
   <si>
     <t>AGE_DIFFERENCE</t>
   </si>
@@ -147,9 +147,6 @@
     <t>Q21C</t>
   </si>
   <si>
-    <t>Q22</t>
-  </si>
-  <si>
     <t>Q25 - Reclassify from 1/2 to 0/1</t>
   </si>
   <si>
@@ -262,6 +259,15 @@
   </si>
   <si>
     <t>Binary</t>
+  </si>
+  <si>
+    <t>q22 removed - handled in how_long_relationship - also laking most data</t>
+  </si>
+  <si>
+    <t>partner_race/respondent_race duplicated</t>
+  </si>
+  <si>
+    <t>dropping this in exchange for PARENTAL_APPROVAL - a binary</t>
   </si>
 </sst>
 </file>
@@ -369,7 +375,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -385,8 +391,26 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -418,11 +442,24 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -430,6 +467,15 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -437,9 +483,162 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA4C2F4"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCC0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA4C2F4"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCC0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA4C2F4"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCC0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA4C2F4"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCC0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA4C2F4"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCC0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE599"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA4C2F4"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCC0000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -793,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63:A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -813,33 +1012,25 @@
       <c r="A2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>79</v>
-      </c>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:4" ht="17" thickBot="1">
       <c r="A3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>80</v>
-      </c>
+      <c r="D3" s="11"/>
     </row>
     <row r="4" spans="1:4" ht="17" thickBot="1">
       <c r="A4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="D4" s="11"/>
     </row>
     <row r="5" spans="1:4" ht="17" thickBot="1">
       <c r="A5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>79</v>
-      </c>
+      <c r="D5" s="11"/>
     </row>
     <row r="6" spans="1:4" ht="17" thickBot="1">
       <c r="A6" s="8" t="s">
@@ -858,7 +1049,7 @@
     </row>
     <row r="9" spans="1:4" ht="17" thickBot="1">
       <c r="A9" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" thickBot="1">
@@ -873,103 +1064,119 @@
     </row>
     <row r="12" spans="1:4" ht="17" thickBot="1">
       <c r="A12" s="8"/>
+      <c r="B12" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="17" thickBot="1">
       <c r="A13" s="8"/>
     </row>
     <row r="14" spans="1:4" ht="17" thickBot="1">
       <c r="A14" s="2" t="s">
-        <v>71</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" thickBot="1">
-      <c r="A15" s="2" t="s">
-        <v>72</v>
+      <c r="A15" s="5" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" thickBot="1">
-      <c r="A16" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="17" thickBot="1">
-      <c r="A17" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="17" thickBot="1">
+      <c r="A16" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17" thickBot="1">
+      <c r="A17" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17" thickBot="1">
       <c r="A18" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="17" thickBot="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="17" thickBot="1">
       <c r="A19" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="17" thickBot="1">
+        <v>15</v>
+      </c>
+      <c r="D19" s="13"/>
+    </row>
+    <row r="20" spans="1:4" ht="17" thickBot="1">
       <c r="A20" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="17" thickBot="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17" thickBot="1">
       <c r="A21" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" ht="17" thickBot="1">
-      <c r="A22" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" ht="17" thickBot="1">
-      <c r="A23" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" ht="17" thickBot="1">
+        <v>27</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17" thickBot="1">
+      <c r="A22" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="17" thickBot="1">
+      <c r="A23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17" thickBot="1">
       <c r="A24" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" ht="17" thickBot="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17" thickBot="1">
       <c r="A25" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" ht="17" thickBot="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17" thickBot="1">
       <c r="A26" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="17" thickBot="1">
+    <row r="27" spans="1:4" ht="17" thickBot="1">
       <c r="A27" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="17" thickBot="1">
+    <row r="28" spans="1:4" ht="17" thickBot="1">
       <c r="A28" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="17" thickBot="1">
+    <row r="29" spans="1:4" ht="17" thickBot="1">
       <c r="A29" s="5" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" ht="17" thickBot="1">
+      <c r="D29" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="17" thickBot="1">
       <c r="A30" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="17" thickBot="1">
+    <row r="31" spans="1:4" ht="17" thickBot="1">
       <c r="A31" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="17" thickBot="1">
+    <row r="32" spans="1:4" ht="17" thickBot="1">
       <c r="A32" s="5" t="s">
         <v>55</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="17" thickBot="1">
@@ -978,255 +1185,257 @@
       </c>
     </row>
     <row r="34" spans="1:1" ht="17" thickBot="1">
-      <c r="A34" s="5" t="s">
-        <v>57</v>
+      <c r="A34" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="17" thickBot="1">
       <c r="A35" s="2" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="17" thickBot="1">
       <c r="A36" s="2" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="17" thickBot="1">
-      <c r="A37" s="4" t="s">
-        <v>26</v>
+      <c r="A37" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="17" thickBot="1">
-      <c r="A38" s="4" t="s">
-        <v>67</v>
+      <c r="A38" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="17" thickBot="1">
-      <c r="A39" s="4" t="s">
-        <v>68</v>
+      <c r="A39" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="17" thickBot="1">
       <c r="A40" s="4" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="17" thickBot="1">
       <c r="A41" s="4" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="17" thickBot="1">
-      <c r="A42" s="4" t="s">
-        <v>74</v>
+      <c r="A42" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="17" thickBot="1">
       <c r="A43" s="4" t="s">
-        <v>75</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="17" thickBot="1">
-      <c r="A44" s="4" t="s">
-        <v>76</v>
+      <c r="A44" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="17" thickBot="1">
-      <c r="A45" s="1" t="s">
-        <v>0</v>
+      <c r="A45" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="17" thickBot="1">
-      <c r="A46" s="1" t="s">
-        <v>1</v>
+      <c r="A46" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="17" thickBot="1">
-      <c r="A47" s="1" t="s">
-        <v>3</v>
+      <c r="A47" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="17" thickBot="1">
       <c r="A48" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" ht="17" thickBot="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="17" thickBot="1">
       <c r="A49" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" ht="17" thickBot="1">
-      <c r="A50" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" ht="17" thickBot="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="17" thickBot="1">
+      <c r="A50" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="17" thickBot="1">
       <c r="A51" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" ht="17" thickBot="1">
-      <c r="A52" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" ht="17" thickBot="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="17" thickBot="1">
+      <c r="A52" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="17" thickBot="1">
       <c r="A53" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" ht="17" thickBot="1">
-      <c r="A54" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" ht="17" thickBot="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="17" thickBot="1">
+      <c r="A54" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="17" thickBot="1">
       <c r="A55" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" ht="17" thickBot="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="17" thickBot="1">
       <c r="A56" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" ht="17" thickBot="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="17" thickBot="1">
       <c r="A57" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" ht="17" thickBot="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="17" thickBot="1">
       <c r="A58" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" ht="17" thickBot="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="17" thickBot="1">
       <c r="A59" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" ht="17" thickBot="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="17" thickBot="1">
       <c r="A60" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" ht="17" thickBot="1">
-      <c r="A61" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" ht="17" thickBot="1">
-      <c r="A62" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" ht="17" thickBot="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="17" thickBot="1">
+      <c r="A61" s="4"/>
+    </row>
+    <row r="62" spans="1:2" ht="17" thickBot="1">
+      <c r="A62" s="4"/>
+      <c r="B62" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="17" thickBot="1">
       <c r="A63" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="17" thickBot="1">
+    <row r="64" spans="1:2" ht="17" thickBot="1">
       <c r="A64" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="17" thickBot="1">
+    <row r="65" spans="1:2" ht="17" thickBot="1">
       <c r="A65" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="17" thickBot="1">
+    <row r="66" spans="1:2" ht="17" thickBot="1">
       <c r="A66" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="17" thickBot="1">
+    <row r="67" spans="1:2" ht="17" thickBot="1">
       <c r="A67" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" ht="17" thickBot="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="17" thickBot="1">
       <c r="A68" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" ht="17" thickBot="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="17" thickBot="1">
       <c r="A69" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="17" thickBot="1">
+      <c r="A70" s="9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="17" thickBot="1">
-      <c r="A70" s="9" t="s">
+    <row r="71" spans="1:2" ht="17" thickBot="1">
+      <c r="A71" s="9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="17" thickBot="1">
-      <c r="A71" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" ht="17" thickBot="1">
+    <row r="72" spans="1:2" ht="17" thickBot="1">
       <c r="A72" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" ht="17" thickBot="1">
+      <c r="B72" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="17" thickBot="1">
       <c r="A73" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="17" thickBot="1">
+      <c r="A74" s="10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="17" thickBot="1">
-      <c r="A74" s="10" t="s">
+    <row r="75" spans="1:2" ht="17" thickBot="1">
+      <c r="A75" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="17" thickBot="1">
-      <c r="A75" s="10" t="s">
+    <row r="76" spans="1:2" ht="17" thickBot="1">
+      <c r="A76" s="10" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="17" thickBot="1">
-      <c r="A76" s="10" t="s">
+    <row r="77" spans="1:2" ht="17" thickBot="1">
+      <c r="A77" s="10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="17" thickBot="1">
-      <c r="A77" s="10" t="s">
+    <row r="78" spans="1:2" ht="17" thickBot="1">
+      <c r="A78" s="10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="17" thickBot="1">
-      <c r="A78" s="10" t="s">
+    <row r="79" spans="1:2" ht="17" thickBot="1">
+      <c r="A79" s="10" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="17" thickBot="1">
-      <c r="A79" s="10" t="s">
+    <row r="80" spans="1:2" ht="17" thickBot="1">
+      <c r="A80" s="9" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" ht="17" thickBot="1">
-      <c r="A80" s="9" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="81" spans="1:1" ht="17" thickBot="1">
       <c r="A81" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="82" spans="1:1" ht="17" thickBot="1">
       <c r="A82" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:A82">
-    <sortCondition sortBy="cellColor" ref="A1:A82" dxfId="2"/>
-    <sortCondition sortBy="cellColor" ref="A1:A82" dxfId="1"/>
-    <sortCondition sortBy="cellColor" ref="A1:A82" dxfId="0"/>
+  <sortState ref="A1:B82">
+    <sortCondition sortBy="cellColor" ref="A1:A82" dxfId="5"/>
+    <sortCondition sortBy="cellColor" ref="A1:A82" dxfId="4"/>
+    <sortCondition sortBy="cellColor" ref="A1:A82" dxfId="3"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>